<commit_message>
verbs added to resources
</commit_message>
<xml_diff>
--- a/resources/01-02-strong-verbs.xlsx
+++ b/resources/01-02-strong-verbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vvj0003/projects/education/deutsch/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347EBB2A-69E2-F34D-847A-163C74ECACCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4AEA35-A28F-0046-8A03-366CB4C446FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="440" windowWidth="16800" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="440" windowWidth="19200" windowHeight="21160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verbs" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Verbs!$A$1:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Verbs!$A$1:$J$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Sie</t>
   </si>
@@ -202,6 +202,30 @@
   </si>
   <si>
     <t>könnt</t>
+  </si>
+  <si>
+    <t>sein</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>bist</t>
+  </si>
+  <si>
+    <t>ist</t>
+  </si>
+  <si>
+    <t>sind</t>
+  </si>
+  <si>
+    <t>seid</t>
+  </si>
+  <si>
+    <t>to be</t>
+  </si>
+  <si>
+    <t>zain</t>
   </si>
 </sst>
 </file>
@@ -451,8 +475,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15FB47A6-AE4F-6D4C-A536-2954825B74E1}" name="Table1" displayName="Table1" ref="A1:J3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:J3" xr:uid="{44931CFB-BC3A-3F4E-96BD-263CD9705C08}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15FB47A6-AE4F-6D4C-A536-2954825B74E1}" name="Table1" displayName="Table1" ref="A1:J4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:J4" xr:uid="{44931CFB-BC3A-3F4E-96BD-263CD9705C08}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -793,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -902,6 +926,38 @@
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>